<commit_message>
Updated README, added data reference. Update setup script, added model results to git.
</commit_message>
<xml_diff>
--- a/notebooks/bottstrapped_metrics_stats.xlsx
+++ b/notebooks/bottstrapped_metrics_stats.xlsx
@@ -593,40 +593,40 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.792</v>
+        <v>0.793</v>
       </c>
       <c r="D4" t="n">
-        <v>0.759</v>
+        <v>0.781</v>
       </c>
       <c r="E4" t="n">
-        <v>0.862</v>
+        <v>0.833</v>
       </c>
       <c r="F4" t="n">
-        <v>0.883</v>
+        <v>0.882</v>
       </c>
       <c r="G4" t="n">
-        <v>0.735</v>
+        <v>0.733</v>
       </c>
       <c r="H4" t="n">
         <v>0.717</v>
       </c>
       <c r="I4" t="n">
-        <v>0.791</v>
+        <v>0.788</v>
       </c>
       <c r="J4" t="n">
+        <v>0.8159999999999999</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.747</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.6909999999999999</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.852</v>
+      </c>
+      <c r="N4" t="n">
         <v>0.82</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.746</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0.672</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0.876</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0.8149999999999999</v>
       </c>
     </row>
     <row r="5">
@@ -637,40 +637,40 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.8090000000000001</v>
+        <v>0.802</v>
       </c>
       <c r="D5" t="n">
-        <v>0.73</v>
+        <v>0.756</v>
       </c>
       <c r="E5" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.869</v>
       </c>
       <c r="F5" t="n">
-        <v>0.895</v>
+        <v>0.887</v>
       </c>
       <c r="G5" t="n">
-        <v>0.738</v>
+        <v>0.736</v>
       </c>
       <c r="H5" t="n">
-        <v>0.721</v>
+        <v>0.719</v>
       </c>
       <c r="I5" t="n">
-        <v>0.791</v>
+        <v>0.852</v>
       </c>
       <c r="J5" t="n">
-        <v>0.821</v>
+        <v>0.8129999999999999</v>
       </c>
       <c r="K5" t="n">
-        <v>0.753</v>
+        <v>0.758</v>
       </c>
       <c r="L5" t="n">
-        <v>0.638</v>
+        <v>0.649</v>
       </c>
       <c r="M5" t="n">
-        <v>0.9399999999999999</v>
+        <v>0.928</v>
       </c>
       <c r="N5" t="n">
-        <v>0.82</v>
+        <v>0.829</v>
       </c>
     </row>
     <row r="6">
@@ -681,40 +681,40 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.048</v>
+        <v>0.049</v>
       </c>
       <c r="D6" t="n">
-        <v>0.079</v>
+        <v>0.082</v>
       </c>
       <c r="E6" t="n">
-        <v>0.145</v>
+        <v>0.131</v>
       </c>
       <c r="F6" t="n">
+        <v>0.035</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.067</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.08799999999999999</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.162</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.057</v>
+      </c>
+      <c r="K6" t="n">
         <v>0.034</v>
       </c>
-      <c r="G6" t="n">
-        <v>0.068</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.092</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.157</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.035</v>
-      </c>
       <c r="L6" t="n">
-        <v>0.08</v>
+        <v>0.083</v>
       </c>
       <c r="M6" t="n">
-        <v>0.135</v>
+        <v>0.142</v>
       </c>
       <c r="N6" t="n">
-        <v>0.035</v>
+        <v>0.031</v>
       </c>
     </row>
   </sheetData>
@@ -782,7 +782,7 @@
         <v>0.7774</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8048</v>
+        <v>0.8057</v>
       </c>
     </row>
     <row r="3">
@@ -800,10 +800,10 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.737</v>
+        <v>0.7578</v>
       </c>
       <c r="E3" t="n">
-        <v>0.7814</v>
+        <v>0.8026</v>
       </c>
     </row>
     <row r="4">
@@ -821,10 +821,10 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0.8183</v>
+        <v>0.795</v>
       </c>
       <c r="E4" t="n">
-        <v>0.9015</v>
+        <v>0.8698</v>
       </c>
     </row>
     <row r="5">
@@ -842,10 +842,10 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.8729</v>
+        <v>0.8715000000000001</v>
       </c>
       <c r="E5" t="n">
-        <v>0.8922</v>
+        <v>0.8921</v>
       </c>
     </row>
     <row r="6">
@@ -863,10 +863,10 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.7355</v>
+        <v>0.737</v>
       </c>
       <c r="E6" t="n">
-        <v>0.7544999999999999</v>
+        <v>0.7564</v>
       </c>
     </row>
     <row r="7">
@@ -884,10 +884,10 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.6501</v>
+        <v>0.6699000000000001</v>
       </c>
       <c r="E7" t="n">
-        <v>0.6958</v>
+        <v>0.715</v>
       </c>
     </row>
     <row r="8">
@@ -905,10 +905,10 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>0.8343</v>
+        <v>0.8099</v>
       </c>
       <c r="E8" t="n">
-        <v>0.9126</v>
+        <v>0.8892</v>
       </c>
     </row>
     <row r="9">
@@ -926,10 +926,10 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>0.8058</v>
+        <v>0.8107</v>
       </c>
       <c r="E9" t="n">
-        <v>0.8243</v>
+        <v>0.8283</v>
       </c>
     </row>
     <row r="10">
@@ -947,10 +947,10 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.7159</v>
+        <v>0.7147</v>
       </c>
       <c r="E10" t="n">
-        <v>0.7542</v>
+        <v>0.7519</v>
       </c>
     </row>
     <row r="11">
@@ -968,10 +968,10 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.6911</v>
+        <v>0.694</v>
       </c>
       <c r="E11" t="n">
-        <v>0.7413999999999999</v>
+        <v>0.739</v>
       </c>
     </row>
     <row r="12">
@@ -989,10 +989,10 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.7455000000000001</v>
+        <v>0.7413</v>
       </c>
       <c r="E12" t="n">
-        <v>0.8338</v>
+        <v>0.8297</v>
       </c>
     </row>
     <row r="13">
@@ -1010,10 +1010,10 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.8026</v>
+        <v>0.8006</v>
       </c>
       <c r="E13" t="n">
-        <v>0.8367</v>
+        <v>0.8322000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>